<commit_message>
cleaning before temporary tracking ignore of xlsx is put in place
</commit_message>
<xml_diff>
--- a/Experiment_Database.xlsx
+++ b/Experiment_Database.xlsx
@@ -817,8 +817,8 @@
     <col min="21" max="21" width="13.09765625" style="15" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6.19921875" style="15" customWidth="1"/>
     <col min="23" max="23" width="23.69921875" style="15" bestFit="1" customWidth="1"/>
-    <col min="24" max="157" width="9.09765625" style="1" customWidth="1"/>
-    <col min="158" max="16384" width="9.09765625" style="1"/>
+    <col min="24" max="158" width="9.09765625" style="1" customWidth="1"/>
+    <col min="159" max="16384" width="9.09765625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">

</xml_diff>